<commit_message>
📝 Fixed "Definition" typo
</commit_message>
<xml_diff>
--- a/Report/Sections/Glossary.xlsx
+++ b/Report/Sections/Glossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\Report\Sections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91252161-2619-4F18-AB1A-BB1D4F15E197}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3302C4DA-5BF6-492D-BD22-6DA09DDAB711}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Defination</t>
-  </si>
-  <si>
     <t>Concept</t>
   </si>
   <si>
@@ -1704,9 +1701,6 @@
     </r>
   </si>
   <si>
-    <t>operation</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Prevent a </t>
     </r>
@@ -1802,6 +1796,12 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Definition</t>
   </si>
 </sst>
 </file>
@@ -2151,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D49:D50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,7 +2171,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -2190,7 +2190,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -2201,10 +2201,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2215,37 +2215,37 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -2253,153 +2253,142 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>44</v>
@@ -2407,288 +2396,299 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="C48" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>